<commit_message>
Case buttons design updated and BOM modification (4.7k R pullup)
</commit_message>
<xml_diff>
--- a/Files for PCBWAY/BOM GNUVario-E V3.1.xlsx
+++ b/Files for PCBWAY/BOM GNUVario-E V3.1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t xml:space="preserve">GNUVario-E V3.1</t>
   </si>
@@ -185,13 +185,19 @@
     <t xml:space="preserve">D_SOD-123</t>
   </si>
   <si>
-    <t xml:space="preserve">R5,R1,R3,R4,R6,R7,R2</t>
+    <t xml:space="preserve">R5,R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 4,7K 0603 1% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1,R3,R4,R7,R2</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor 10K 0603 1% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R_0603_1608Metric</t>
   </si>
   <si>
     <t xml:space="preserve">R8</t>
@@ -246,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -319,6 +325,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -388,7 +400,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -439,6 +451,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -524,11 +540,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>9360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>661680</xdr:colOff>
+      <xdr:colOff>661320</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
@@ -543,8 +559,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9360" y="211680"/>
-          <a:ext cx="1280880" cy="371160"/>
+          <a:off x="9360" y="212040"/>
+          <a:ext cx="1280520" cy="370800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -567,7 +583,7 @@
   <dimension ref="A2:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,11 +800,11 @@
         <v>27</v>
       </c>
       <c r="C13" s="8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="13" t="s">
         <v>28</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -803,11 +819,11 @@
       <c r="A14" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="12"/>
@@ -826,50 +842,46 @@
       <c r="A15" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>35</v>
+      <c r="G15" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>13</v>
@@ -881,34 +893,54 @@
         <v>11</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="8" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
@@ -1176,12 +1208,18 @@
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+    </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>